<commit_message>
change the normalization for 10002 and 20002
</commit_message>
<xml_diff>
--- a/pp_hadron/expdata/10002.xlsx
+++ b/pp_hadron/expdata/10002.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17700"/>
+    <workbookView windowHeight="17960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
     <t>pion_+-</t>
   </si>
   <si>
-    <t>d2N/N_inel-dy-dpt</t>
+    <t>d2N/N_vis-dy-dpt</t>
   </si>
   <si>
     <t>pb</t>
@@ -82,30 +82,68 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -113,96 +151,45 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -210,23 +197,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -234,7 +205,36 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -248,7 +248,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,175 +416,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,45 +439,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -505,6 +466,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -522,15 +492,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -539,153 +500,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -701,55 +701,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1026,12 +1026,12 @@
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="3" max="3" width="10.25" customWidth="1"/>
-    <col min="4" max="4" width="10.5625" customWidth="1"/>
-    <col min="11" max="11" width="16.25" customWidth="1"/>
-    <col min="13" max="15" width="12.6875"/>
+    <col min="4" max="4" width="10.5673076923077" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="13" max="15" width="12.6923076923077"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">

</xml_diff>